<commit_message>
Added EFC and Amt Borrowed plots
</commit_message>
<xml_diff>
--- a/efc_and_amt_borrowed_over_time.xlsx
+++ b/efc_and_amt_borrowed_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolan/MACALESTER/Stat 456/stat456_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3479C1F0-42D6-2240-B2A6-30BEFE6D72C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8389AB90-5349-374C-975F-206EF6CC5A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0DCA1C52-C746-644D-892B-BD6C0B874043}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="18">
   <si>
     <t>Field of study: undergraduate (10 categories)</t>
   </si>
@@ -90,25 +90,13 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>Undeclared</t>
-  </si>
-  <si>
-    <t>Bio and phys science, sci tech, math, agriculture</t>
-  </si>
-  <si>
-    <t>Social Sciences</t>
-  </si>
-  <si>
-    <t>Other Applied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,13 +106,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,11 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -481,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AEAE09-117A-CA45-8FF6-F5F367835651}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:E67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,21 +485,21 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>8897.7999999999993</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>3137.4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>2016</v>
       </c>
       <c r="E2" t="s">
@@ -528,16 +507,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>9666</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>9614.2000000000007</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>2016</v>
       </c>
       <c r="E3" t="s">
@@ -545,16 +524,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>12798.6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>8703</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>2016</v>
       </c>
       <c r="E4" t="s">
@@ -562,16 +541,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>15905.3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>9057.9</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>2016</v>
       </c>
       <c r="E5" t="s">
@@ -579,16 +558,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>10936.1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>5324.4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>2016</v>
       </c>
       <c r="E6" t="s">
@@ -596,16 +575,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>12906.9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>10874</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>2016</v>
       </c>
       <c r="E7" t="s">
@@ -613,16 +592,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>13199.7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>11119.7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>2016</v>
       </c>
       <c r="E8" t="s">
@@ -630,16 +609,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>8745.4</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>11015.2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>2016</v>
       </c>
       <c r="E9" t="s">
@@ -647,16 +626,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>13060.7</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>9950.2000000000007</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>2016</v>
       </c>
       <c r="E10" t="s">
@@ -664,16 +643,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>10481.5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>9932.4</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>2016</v>
       </c>
       <c r="E11" t="s">
@@ -681,16 +660,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>8739.2000000000007</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>9152.7000000000007</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>2016</v>
       </c>
       <c r="E12" t="s">
@@ -698,937 +677,937 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>8123.5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1">
         <v>4872</v>
       </c>
-      <c r="D13" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13">
+        <v>2016</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>8090.3</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1">
         <v>11082.7</v>
       </c>
-      <c r="D14" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14">
+        <v>2016</v>
+      </c>
+      <c r="E14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>13878.3</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
         <v>9459.1</v>
       </c>
-      <c r="D15" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15">
+        <v>2016</v>
+      </c>
+      <c r="E15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>13515.9</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
         <v>9674</v>
       </c>
-      <c r="D16" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16">
+        <v>2016</v>
+      </c>
+      <c r="E16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>8745.5</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
         <v>7324</v>
       </c>
-      <c r="D17" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17">
+        <v>2016</v>
+      </c>
+      <c r="E17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="1">
         <v>9038.2000000000007</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1">
         <v>13304.4</v>
       </c>
-      <c r="D18" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18">
+        <v>2016</v>
+      </c>
+      <c r="E18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <v>12725.5</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
         <v>10519.4</v>
       </c>
-      <c r="D19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D19">
+        <v>2016</v>
+      </c>
+      <c r="E19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>6738.3</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
         <v>12995.3</v>
       </c>
-      <c r="D20" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20">
+        <v>2016</v>
+      </c>
+      <c r="E20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="1">
         <v>9888</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1">
         <v>12608.2</v>
       </c>
-      <c r="D21" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21">
+        <v>2016</v>
+      </c>
+      <c r="E21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="1">
         <v>8163.5</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1">
         <v>10558.2</v>
       </c>
-      <c r="D22" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D22">
+        <v>2016</v>
+      </c>
+      <c r="E22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="1">
         <v>8269.1</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="1">
         <v>12021.8</v>
       </c>
-      <c r="D23" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="D23">
+        <v>2016</v>
+      </c>
+      <c r="E23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>10643.8</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="1">
         <v>5386.1</v>
       </c>
-      <c r="D24" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="D24">
+        <v>2012</v>
+      </c>
+      <c r="E24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>7386.5</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="1">
         <v>9805.2999999999993</v>
       </c>
-      <c r="D25" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25">
+        <v>2012</v>
+      </c>
+      <c r="E25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="1">
         <v>9986.7999999999993</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="1">
         <v>8403</v>
       </c>
-      <c r="D26" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26">
+        <v>2012</v>
+      </c>
+      <c r="E26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="1">
         <v>11058.1</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="1">
         <v>9690.1</v>
       </c>
-      <c r="D27" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27">
+        <v>2012</v>
+      </c>
+      <c r="E27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="1">
         <v>8424.1</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="1">
         <v>4053.3</v>
       </c>
-      <c r="D28" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="D28">
+        <v>2012</v>
+      </c>
+      <c r="E28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>11250.8</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="1">
         <v>10743.7</v>
       </c>
-      <c r="D29" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D29">
+        <v>2012</v>
+      </c>
+      <c r="E29" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="1">
         <v>9874.5</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="1">
         <v>10854.4</v>
       </c>
-      <c r="D30" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30">
+        <v>2012</v>
+      </c>
+      <c r="E30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="1">
         <v>6620.3</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="1">
         <v>8554.4</v>
       </c>
-      <c r="D31" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31">
+        <v>2012</v>
+      </c>
+      <c r="E31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="1">
         <v>9767.7000000000007</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="1">
         <v>9639.9</v>
       </c>
-      <c r="D32" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32">
+        <v>2012</v>
+      </c>
+      <c r="E32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="1">
         <v>7843.8</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="1">
         <v>12706.9</v>
       </c>
-      <c r="D33" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="D33">
+        <v>2012</v>
+      </c>
+      <c r="E33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="1">
         <v>7325.4</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="1">
         <v>9255.9</v>
       </c>
-      <c r="D34" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D34">
+        <v>2012</v>
+      </c>
+      <c r="E34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="1">
         <v>9928.5</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="1">
         <v>5738.6</v>
       </c>
-      <c r="D35" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="D35">
+        <v>2012</v>
+      </c>
+      <c r="E35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="1">
         <v>7468.7</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="1">
         <v>11383.2</v>
       </c>
-      <c r="D36" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="D36">
+        <v>2012</v>
+      </c>
+      <c r="E36" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="1">
         <v>11567.8</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="1">
         <v>10877</v>
       </c>
-      <c r="D37" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="D37">
+        <v>2012</v>
+      </c>
+      <c r="E37" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="1">
         <v>11620.7</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="1">
         <v>9849.2000000000007</v>
       </c>
-      <c r="D38" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="D38">
+        <v>2012</v>
+      </c>
+      <c r="E38" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>6520.6</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="1">
         <v>5865.7</v>
       </c>
-      <c r="D39" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="D39">
+        <v>2012</v>
+      </c>
+      <c r="E39" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>8719.7000000000007</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="1">
         <v>13307.1</v>
       </c>
-      <c r="D40" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="D40">
+        <v>2012</v>
+      </c>
+      <c r="E40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="1">
         <v>10960.9</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="1">
         <v>10939.3</v>
       </c>
-      <c r="D41" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="D41">
+        <v>2012</v>
+      </c>
+      <c r="E41" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="1">
         <v>5987.5</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="1">
         <v>10813.7</v>
       </c>
-      <c r="D42" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="D42">
+        <v>2012</v>
+      </c>
+      <c r="E42" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="1">
         <v>7200.5</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="1">
         <v>12124.1</v>
       </c>
-      <c r="D43" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="D43">
+        <v>2012</v>
+      </c>
+      <c r="E43" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="1">
         <v>8092.7</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="1">
         <v>10665.8</v>
       </c>
-      <c r="D44" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="D44">
+        <v>2012</v>
+      </c>
+      <c r="E44" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="1">
         <v>6853.7</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="1">
         <v>11925.6</v>
       </c>
-      <c r="D45" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="D45">
+        <v>2012</v>
+      </c>
+      <c r="E45" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="3">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1">
         <v>10748</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="1">
         <v>3250.5</v>
       </c>
-      <c r="D46" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="D46">
+        <v>2008</v>
+      </c>
+      <c r="E46" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="1">
         <v>9098.4</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="1">
         <v>7137.9</v>
       </c>
-      <c r="D47" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="D47">
+        <v>2008</v>
+      </c>
+      <c r="E47" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="1">
         <v>11512.3</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="1">
         <v>6814.7</v>
       </c>
-      <c r="D48" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="D48">
+        <v>2008</v>
+      </c>
+      <c r="E48" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="3">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
         <v>12257.2</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="1">
         <v>7257.1</v>
       </c>
-      <c r="D49" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E49" s="1" t="s">
+      <c r="D49">
+        <v>2008</v>
+      </c>
+      <c r="E49" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="1">
         <v>10092.9</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="1">
         <v>3407</v>
       </c>
-      <c r="D50" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E50" s="1" t="s">
+      <c r="D50">
+        <v>2008</v>
+      </c>
+      <c r="E50" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="3">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1">
         <v>13304.9</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="1">
         <v>9378.9</v>
       </c>
-      <c r="D51" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="D51">
+        <v>2008</v>
+      </c>
+      <c r="E51" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="1">
         <v>12191.4</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="1">
         <v>9441.1</v>
       </c>
-      <c r="D52" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="D52">
+        <v>2008</v>
+      </c>
+      <c r="E52" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="1">
         <v>8380.9</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="1">
         <v>7132.4</v>
       </c>
-      <c r="D53" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="D53">
+        <v>2008</v>
+      </c>
+      <c r="E53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="1">
         <v>12246.7</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="1">
         <v>7428.9</v>
       </c>
-      <c r="D54" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="D54">
+        <v>2008</v>
+      </c>
+      <c r="E54" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="1">
         <v>9204.9</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="1">
         <v>8049.3</v>
       </c>
-      <c r="D55" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="D55">
+        <v>2008</v>
+      </c>
+      <c r="E55" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="3">
+      <c r="A56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="1">
         <v>9919.7000000000007</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="1">
         <v>6547.5</v>
       </c>
-      <c r="D56" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="D56">
+        <v>2008</v>
+      </c>
+      <c r="E56" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="B57">
         <v>8989.9</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
         <v>3883</v>
       </c>
-      <c r="D57" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="D57">
+        <v>2008</v>
+      </c>
+      <c r="E57" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58">
         <v>7401.7</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
         <v>8360.6</v>
       </c>
-      <c r="D58" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="D58">
+        <v>2008</v>
+      </c>
+      <c r="E58" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59">
         <v>11626.9</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
         <v>8278.2000000000007</v>
       </c>
-      <c r="D59" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="D59">
+        <v>2008</v>
+      </c>
+      <c r="E59" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="1">
+        <v>4</v>
+      </c>
+      <c r="B60">
         <v>11315.4</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
         <v>7689.1</v>
       </c>
-      <c r="D60" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="D60">
+        <v>2008</v>
+      </c>
+      <c r="E60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>9367.2999999999993</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
         <v>4656.2</v>
       </c>
-      <c r="D61" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="D61">
+        <v>2008</v>
+      </c>
+      <c r="E61" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" s="1">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62">
         <v>11318.5</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
         <v>10205.1</v>
       </c>
-      <c r="D62" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="D62">
+        <v>2008</v>
+      </c>
+      <c r="E62" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
         <v>12377.1</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
         <v>9290</v>
       </c>
-      <c r="D63" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="D63">
+        <v>2008</v>
+      </c>
+      <c r="E63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
         <v>6629.9</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
         <v>7998</v>
       </c>
-      <c r="D64" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="D64">
+        <v>2008</v>
+      </c>
+      <c r="E64" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>9375.2000000000007</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>9106.5</v>
       </c>
-      <c r="D65" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="D65">
+        <v>2008</v>
+      </c>
+      <c r="E65" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
         <v>9581.1</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66">
         <v>8091.8</v>
       </c>
-      <c r="D66" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="D66">
+        <v>2008</v>
+      </c>
+      <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="1">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67">
         <v>9085</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67">
         <v>8682.2999999999993</v>
       </c>
-      <c r="D67" s="1">
-        <v>2008</v>
-      </c>
-      <c r="E67" s="1" t="s">
+      <c r="D67">
+        <v>2008</v>
+      </c>
+      <c r="E67" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>